<commit_message>
feat:collected responses with corrected grammar
</commit_message>
<xml_diff>
--- a/06-08-2023/data/output/xlsx/sample_0/10_causality.xlsx
+++ b/06-08-2023/data/output/xlsx/sample_0/10_causality.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="125">
   <si>
     <t>name</t>
   </si>
@@ -334,25 +334,61 @@
     <t>n/a</t>
   </si>
   <si>
-    <t>num_of_adds_and_subs__1,num_of_equals__0,num_of_equals__1,num_of_unknowns__1,num_of_unknowns__10,num_of_unknowns__9</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__0,num_of_equals__0,num_of_equals__1,num_of_unknowns__1,num_of_unknowns__10,num_of_unknowns__9</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_equals__1,num_of_unknowns__1,num_of_unknowns__10,num_of_unknowns__9</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_equals__0,num_of_unknowns__1,num_of_unknowns__10,num_of_unknowns__9</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_equals__0,num_of_equals__1,num_of_unknowns__10,num_of_unknowns__9</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_equals__0,num_of_equals__1,num_of_unknowns__1,num_of_unknowns__9</t>
-  </si>
-  <si>
-    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_equals__0,num_of_equals__1,num_of_unknowns__1,num_of_unknowns__10</t>
+    <t>num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_decimals__0,num_of_equals__0,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_unknowns__1,num_of_unknowns__2,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_decimals__0,num_of_equals__0,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_unknowns__1,num_of_unknowns__2,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_decimals__0,num_of_equals__0,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_unknowns__1,num_of_unknowns__2,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_decimals__0,num_of_equals__0,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_unknowns__1,num_of_unknowns__2,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__5,num_of_decimals__0,num_of_equals__0,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_unknowns__1,num_of_unknowns__2,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_decimals__0,num_of_equals__0,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_unknowns__1,num_of_unknowns__2,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_equals__0,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_unknowns__1,num_of_unknowns__2,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_decimals__0,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_unknowns__1,num_of_unknowns__2,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_decimals__0,num_of_equals__0,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_unknowns__1,num_of_unknowns__2,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_decimals__0,num_of_equals__0,num_of_equals__1,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_unknowns__1,num_of_unknowns__2,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_decimals__0,num_of_equals__0,num_of_equals__1,num_of_equals__2,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_unknowns__1,num_of_unknowns__2,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_decimals__0,num_of_equals__0,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__5,num_of_equals__6,num_of_unknowns__1,num_of_unknowns__2,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_decimals__0,num_of_equals__0,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__6,num_of_unknowns__1,num_of_unknowns__2,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_decimals__0,num_of_equals__0,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_unknowns__1,num_of_unknowns__2,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_decimals__0,num_of_equals__0,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_unknowns__2,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_decimals__0,num_of_equals__0,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_unknowns__1,pairs_of_parentheses__0,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_decimals__0,num_of_equals__0,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_unknowns__1,num_of_unknowns__2,pairs_of_parentheses__1,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_decimals__0,num_of_equals__0,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_unknowns__1,num_of_unknowns__2,pairs_of_parentheses__0,pairs_of_parentheses__2</t>
+  </si>
+  <si>
+    <t>num_of_adds_and_subs__0,num_of_adds_and_subs__1,num_of_adds_and_subs__2,num_of_adds_and_subs__3,num_of_adds_and_subs__4,num_of_adds_and_subs__5,num_of_decimals__0,num_of_equals__0,num_of_equals__1,num_of_equals__2,num_of_equals__3,num_of_equals__4,num_of_equals__5,num_of_equals__6,num_of_unknowns__1,num_of_unknowns__2,pairs_of_parentheses__0,pairs_of_parentheses__1</t>
   </si>
 </sst>
 </file>
@@ -750,19 +786,19 @@
         <v>968</v>
       </c>
       <c r="D2">
-        <v>7.229453571447539</v>
+        <v>0.003930642998268821</v>
       </c>
       <c r="E2" t="s">
         <v>106</v>
       </c>
       <c r="F2">
-        <v>11.06198347107438</v>
+        <v>0.001033057851239669</v>
       </c>
       <c r="G2">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H2">
-        <v>0.0609814670663642</v>
+        <v>3.105384322363747E-05</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -776,19 +812,19 @@
         <v>835</v>
       </c>
       <c r="D3">
-        <v>4.057166183651596</v>
+        <v>0.0040941325007247</v>
       </c>
       <c r="E3" t="s">
         <v>107</v>
       </c>
       <c r="F3">
-        <v>11.02994011976048</v>
+        <v>0.001197604790419162</v>
       </c>
       <c r="G3">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H3">
-        <v>0.02893811575246197</v>
+        <v>0.0001956007824031297</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -805,13 +841,13 @@
         <v>105</v>
       </c>
       <c r="F4">
-        <v>5.727272727272728</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H4">
-        <v>-5.273729276735289</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -828,13 +864,13 @@
         <v>105</v>
       </c>
       <c r="F5">
-        <v>6.111111111111111</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H5">
-        <v>-4.889890892896906</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -851,13 +887,13 @@
         <v>105</v>
       </c>
       <c r="F6">
-        <v>6.111111111111111</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H6">
-        <v>-4.889890892896906</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -874,13 +910,13 @@
         <v>105</v>
       </c>
       <c r="F7">
-        <v>5.666666666666667</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H7">
-        <v>-5.33433533734135</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -897,13 +933,13 @@
         <v>105</v>
       </c>
       <c r="F8">
-        <v>6.6</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H8">
-        <v>-4.401002004008017</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -920,13 +956,13 @@
         <v>105</v>
       </c>
       <c r="F9">
-        <v>4.75</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H9">
-        <v>-6.251002004008017</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -943,13 +979,13 @@
         <v>105</v>
       </c>
       <c r="F10">
-        <v>5.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H10">
-        <v>-5.667668670674684</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -966,13 +1002,13 @@
         <v>105</v>
       </c>
       <c r="F11">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H11">
-        <v>-3.501002004008017</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -985,17 +1021,20 @@
       <c r="C12">
         <v>427</v>
       </c>
-      <c r="D12" t="s">
-        <v>105</v>
+      <c r="D12">
+        <v>0.005006788809859134</v>
+      </c>
+      <c r="E12" t="s">
+        <v>108</v>
       </c>
       <c r="F12">
-        <v>10.74004683840749</v>
+        <v>0.00234192037470726</v>
       </c>
       <c r="G12">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H12">
-        <v>-0.2609551656005227</v>
+        <v>0.001339916366691228</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1008,17 +1047,20 @@
       <c r="C13">
         <v>295</v>
       </c>
-      <c r="D13" t="s">
-        <v>105</v>
+      <c r="D13">
+        <v>0.006081729027441573</v>
+      </c>
+      <c r="E13" t="s">
+        <v>109</v>
       </c>
       <c r="F13">
-        <v>10.24745762711864</v>
+        <v>0.003389830508474576</v>
       </c>
       <c r="G13">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H13">
-        <v>-0.7535443768893728</v>
+        <v>0.002387826500458544</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1031,17 +1073,20 @@
       <c r="C14">
         <v>175</v>
       </c>
-      <c r="D14" t="s">
-        <v>105</v>
+      <c r="D14">
+        <v>0.008705505449740768</v>
+      </c>
+      <c r="E14" t="s">
+        <v>110</v>
       </c>
       <c r="F14">
-        <v>9.800000000000001</v>
+        <v>0.005714285714285714</v>
       </c>
       <c r="G14">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H14">
-        <v>-1.201002004008016</v>
+        <v>0.004712281706269682</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1054,17 +1099,20 @@
       <c r="C15">
         <v>130</v>
       </c>
-      <c r="D15" t="s">
-        <v>105</v>
+      <c r="D15">
+        <v>0.01072827106703724</v>
+      </c>
+      <c r="E15" t="s">
+        <v>111</v>
       </c>
       <c r="F15">
-        <v>9.699999999999999</v>
+        <v>0.007692307692307693</v>
       </c>
       <c r="G15">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H15">
-        <v>-1.301002004008017</v>
+        <v>0.006690303684291661</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1081,13 +1129,13 @@
         <v>105</v>
       </c>
       <c r="F16">
-        <v>9.858974358974359</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H16">
-        <v>-1.142027645033657</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1104,13 +1152,13 @@
         <v>105</v>
       </c>
       <c r="F17">
-        <v>8.73076923076923</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H17">
-        <v>-2.270232773238787</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1127,13 +1175,13 @@
         <v>105</v>
       </c>
       <c r="F18">
-        <v>7.038461538461538</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H18">
-        <v>-3.962540465546478</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1150,13 +1198,13 @@
         <v>105</v>
       </c>
       <c r="F19">
-        <v>6.176470588235294</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H19">
-        <v>-4.824531415772722</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1169,17 +1217,20 @@
       <c r="C20">
         <v>650</v>
       </c>
-      <c r="D20" t="s">
-        <v>105</v>
+      <c r="D20">
+        <v>0.004865269638079896</v>
+      </c>
+      <c r="E20" t="s">
+        <v>112</v>
       </c>
       <c r="F20">
-        <v>9.813846153846153</v>
+        <v>0.001538461538461538</v>
       </c>
       <c r="G20">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H20">
-        <v>-1.187155850161863</v>
+        <v>0.0005364575304455065</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1196,13 +1247,13 @@
         <v>105</v>
       </c>
       <c r="F21">
-        <v>9.298850574712644</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H21">
-        <v>-1.702151429295373</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1219,13 +1270,13 @@
         <v>105</v>
       </c>
       <c r="F22">
-        <v>8.722222222222221</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H22">
-        <v>-2.278779781785795</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1242,13 +1293,13 @@
         <v>105</v>
       </c>
       <c r="F23">
-        <v>9.555555555555555</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H23">
-        <v>-1.445446448452461</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1265,13 +1316,13 @@
         <v>105</v>
       </c>
       <c r="F24">
-        <v>7.75</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H24">
-        <v>-3.251002004008017</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1288,13 +1339,13 @@
         <v>105</v>
       </c>
       <c r="F25">
-        <v>6.25</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H25">
-        <v>-4.751002004008017</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1311,13 +1362,13 @@
         <v>105</v>
       </c>
       <c r="F26">
-        <v>6.777777777777778</v>
+        <v>0</v>
       </c>
       <c r="G26">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H26">
-        <v>-4.223224226230239</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1334,13 +1385,13 @@
         <v>105</v>
       </c>
       <c r="F27">
-        <v>7.5</v>
+        <v>0</v>
       </c>
       <c r="G27">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H27">
-        <v>-3.501002004008017</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1357,13 +1408,13 @@
         <v>105</v>
       </c>
       <c r="F28">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="G28">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H28">
-        <v>-5.501002004008017</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1380,13 +1431,13 @@
         <v>105</v>
       </c>
       <c r="F29">
-        <v>2.666666666666667</v>
+        <v>0</v>
       </c>
       <c r="G29">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H29">
-        <v>-8.334335337341351</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1403,13 +1454,13 @@
         <v>105</v>
       </c>
       <c r="F30">
-        <v>2.666666666666667</v>
+        <v>0</v>
       </c>
       <c r="G30">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H30">
-        <v>-8.334335337341351</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1426,13 +1477,13 @@
         <v>105</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H31">
-        <v>-10.00100200400802</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1449,13 +1500,13 @@
         <v>105</v>
       </c>
       <c r="F32">
-        <v>9.299270072992702</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H32">
-        <v>-1.701731931015315</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1472,13 +1523,13 @@
         <v>105</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H33">
-        <v>-10.00100200400802</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1495,13 +1546,13 @@
         <v>105</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H34">
-        <v>-10.00100200400802</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1518,13 +1569,13 @@
         <v>105</v>
       </c>
       <c r="F35">
-        <v>8.508250825082508</v>
+        <v>0</v>
       </c>
       <c r="G35">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H35">
-        <v>-2.492751178925509</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1541,13 +1592,13 @@
         <v>105</v>
       </c>
       <c r="F36">
-        <v>8.42512077294686</v>
+        <v>0</v>
       </c>
       <c r="G36">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H36">
-        <v>-2.575881231061157</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1564,13 +1615,13 @@
         <v>105</v>
       </c>
       <c r="F37">
-        <v>8.742331288343559</v>
+        <v>0</v>
       </c>
       <c r="G37">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H37">
-        <v>-2.258670715664458</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1587,13 +1638,13 @@
         <v>105</v>
       </c>
       <c r="F38">
-        <v>8.535714285714286</v>
+        <v>0</v>
       </c>
       <c r="G38">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H38">
-        <v>-2.46528771829373</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1610,13 +1661,13 @@
         <v>105</v>
       </c>
       <c r="F39">
-        <v>8.51685393258427</v>
+        <v>0</v>
       </c>
       <c r="G39">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H39">
-        <v>-2.484148071423746</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1633,13 +1684,13 @@
         <v>105</v>
       </c>
       <c r="F40">
-        <v>7.915254237288136</v>
+        <v>0</v>
       </c>
       <c r="G40">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H40">
-        <v>-3.085747766719881</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1656,13 +1707,13 @@
         <v>105</v>
       </c>
       <c r="F41">
-        <v>7.911111111111111</v>
+        <v>0</v>
       </c>
       <c r="G41">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H41">
-        <v>-3.089890892896905</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1676,19 +1727,19 @@
         <v>996</v>
       </c>
       <c r="D42">
-        <v>10.86093110930142</v>
+        <v>0.003874608011323235</v>
       </c>
       <c r="E42" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="F42">
-        <v>11.01907630522088</v>
+        <v>0.001004016064257028</v>
       </c>
       <c r="G42">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H42">
-        <v>0.01807430121286657</v>
+        <v>2.012056240996039E-06</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1702,19 +1753,19 @@
         <v>991</v>
       </c>
       <c r="D43">
-        <v>5.415386801013085</v>
+        <v>0.003877768051909507</v>
       </c>
       <c r="E43" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="F43">
-        <v>11.029263370333</v>
+        <v>0.001009081735620585</v>
       </c>
       <c r="G43">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H43">
-        <v>0.02826136632497978</v>
+        <v>7.077727604553295E-06</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1731,13 +1782,13 @@
         <v>105</v>
       </c>
       <c r="F44">
-        <v>5.583333333333333</v>
+        <v>0</v>
       </c>
       <c r="G44">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H44">
-        <v>-5.417668670674684</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1754,13 +1805,13 @@
         <v>105</v>
       </c>
       <c r="F45">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="G45">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H45">
-        <v>-8.501002004008017</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1777,13 +1828,13 @@
         <v>105</v>
       </c>
       <c r="F46">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G46">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H46">
-        <v>-7.001002004008017</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1796,17 +1847,20 @@
       <c r="C47">
         <v>649</v>
       </c>
-      <c r="D47" t="s">
-        <v>105</v>
+      <c r="D47">
+        <v>0.004162035505347234</v>
+      </c>
+      <c r="E47" t="s">
+        <v>115</v>
       </c>
       <c r="F47">
-        <v>10.70878274268105</v>
+        <v>0.001540832049306626</v>
       </c>
       <c r="G47">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H47">
-        <v>-0.2922192613269683</v>
+        <v>0.0005388280412905937</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1819,17 +1873,20 @@
       <c r="C48">
         <v>475</v>
       </c>
-      <c r="D48" t="s">
-        <v>105</v>
+      <c r="D48">
+        <v>0.004601669734497333</v>
+      </c>
+      <c r="E48" t="s">
+        <v>116</v>
       </c>
       <c r="F48">
-        <v>10.6021052631579</v>
+        <v>0.002105263157894737</v>
       </c>
       <c r="G48">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H48">
-        <v>-0.3988967408501214</v>
+        <v>0.001103259149878705</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1842,17 +1899,20 @@
       <c r="C49">
         <v>307</v>
       </c>
-      <c r="D49" t="s">
-        <v>105</v>
+      <c r="D49">
+        <v>0.005607672530490811</v>
+      </c>
+      <c r="E49" t="s">
+        <v>117</v>
       </c>
       <c r="F49">
-        <v>10.74918566775244</v>
+        <v>0.003257328990228013</v>
       </c>
       <c r="G49">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H49">
-        <v>-0.2518163362555743</v>
+        <v>0.002255324982211981</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1865,17 +1925,20 @@
       <c r="C50">
         <v>233</v>
       </c>
-      <c r="D50" t="s">
-        <v>105</v>
+      <c r="D50">
+        <v>0.006534190002533634</v>
+      </c>
+      <c r="E50" t="s">
+        <v>118</v>
       </c>
       <c r="F50">
-        <v>10.54077253218884</v>
+        <v>0.004291845493562232</v>
       </c>
       <c r="G50">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H50">
-        <v>-0.4602294718191757</v>
+        <v>0.0032898414855462</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1888,17 +1951,20 @@
       <c r="C51">
         <v>154</v>
       </c>
-      <c r="D51" t="s">
-        <v>105</v>
+      <c r="D51">
+        <v>0.008832018144092381</v>
+      </c>
+      <c r="E51" t="s">
+        <v>119</v>
       </c>
       <c r="F51">
-        <v>10.14935064935065</v>
+        <v>0.006493506493506494</v>
       </c>
       <c r="G51">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H51">
-        <v>-0.851651354657367</v>
+        <v>0.005491502485490462</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1915,13 +1981,13 @@
         <v>105</v>
       </c>
       <c r="F52">
-        <v>10.26732673267327</v>
+        <v>0</v>
       </c>
       <c r="G52">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H52">
-        <v>-0.7336752713347501</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1938,13 +2004,13 @@
         <v>105</v>
       </c>
       <c r="F53">
-        <v>10.03225806451613</v>
+        <v>0</v>
       </c>
       <c r="G53">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H53">
-        <v>-0.9687439394918869</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1961,13 +2027,13 @@
         <v>105</v>
       </c>
       <c r="F54">
-        <v>8.1</v>
+        <v>0</v>
       </c>
       <c r="G54">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H54">
-        <v>-2.901002004008017</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1984,13 +2050,13 @@
         <v>105</v>
       </c>
       <c r="F55">
-        <v>7.791666666666667</v>
+        <v>0</v>
       </c>
       <c r="G55">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H55">
-        <v>-3.20933533734135</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2007,13 +2073,13 @@
         <v>105</v>
       </c>
       <c r="F56">
-        <v>7.730994152046784</v>
+        <v>0</v>
       </c>
       <c r="G56">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H56">
-        <v>-3.270007851961233</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2030,13 +2096,13 @@
         <v>105</v>
       </c>
       <c r="F57">
-        <v>4.888888888888889</v>
+        <v>0</v>
       </c>
       <c r="G57">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H57">
-        <v>-6.112113115119127</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -2053,13 +2119,13 @@
         <v>105</v>
       </c>
       <c r="F58">
-        <v>5.375</v>
+        <v>0</v>
       </c>
       <c r="G58">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H58">
-        <v>-5.626002004008017</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -2076,13 +2142,13 @@
         <v>105</v>
       </c>
       <c r="F59">
-        <v>6.5</v>
+        <v>0</v>
       </c>
       <c r="G59">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H59">
-        <v>-4.501002004008017</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2099,13 +2165,13 @@
         <v>105</v>
       </c>
       <c r="F60">
-        <v>6.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="G60">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H60">
-        <v>-4.667668670674684</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2122,13 +2188,13 @@
         <v>105</v>
       </c>
       <c r="F61">
-        <v>6.333333333333333</v>
+        <v>0</v>
       </c>
       <c r="G61">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H61">
-        <v>-4.667668670674684</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2145,13 +2211,13 @@
         <v>105</v>
       </c>
       <c r="F62">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G62">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H62">
-        <v>-6.001002004008017</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2168,13 +2234,13 @@
         <v>105</v>
       </c>
       <c r="F63">
-        <v>7.445454545454545</v>
+        <v>0</v>
       </c>
       <c r="G63">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H63">
-        <v>-3.555547458553471</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2191,13 +2257,13 @@
         <v>105</v>
       </c>
       <c r="F64">
-        <v>7.709677419354839</v>
+        <v>0</v>
       </c>
       <c r="G64">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H64">
-        <v>-3.291324584653178</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2214,13 +2280,13 @@
         <v>105</v>
       </c>
       <c r="F65">
-        <v>7.27536231884058</v>
+        <v>0</v>
       </c>
       <c r="G65">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H65">
-        <v>-3.725639685167437</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2237,13 +2303,13 @@
         <v>105</v>
       </c>
       <c r="F66">
-        <v>7.150943396226415</v>
+        <v>0</v>
       </c>
       <c r="G66">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H66">
-        <v>-3.850058607781602</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2260,13 +2326,13 @@
         <v>105</v>
       </c>
       <c r="F67">
-        <v>7.28125</v>
+        <v>0</v>
       </c>
       <c r="G67">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H67">
-        <v>-3.719752004008017</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2283,13 +2349,13 @@
         <v>105</v>
       </c>
       <c r="F68">
-        <v>5.96</v>
+        <v>0</v>
       </c>
       <c r="G68">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H68">
-        <v>-5.041002004008017</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2306,13 +2372,13 @@
         <v>105</v>
       </c>
       <c r="F69">
-        <v>5.823529411764706</v>
+        <v>0</v>
       </c>
       <c r="G69">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H69">
-        <v>-5.177472592243311</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2329,13 +2395,13 @@
         <v>105</v>
       </c>
       <c r="F70">
-        <v>5.545454545454546</v>
+        <v>0</v>
       </c>
       <c r="G70">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H70">
-        <v>-5.455547458553471</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2352,10 +2418,10 @@
         <v>105</v>
       </c>
       <c r="F71">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="G71">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -2372,19 +2438,19 @@
         <v>708</v>
       </c>
       <c r="D72">
-        <v>4.036060392289436</v>
+        <v>0.004505171514961335</v>
       </c>
       <c r="E72" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="F72">
-        <v>11.00847457627119</v>
+        <v>0.001412429378531073</v>
       </c>
       <c r="G72">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H72">
-        <v>0.007472572263170107</v>
+        <v>0.0004104253705150415</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2397,20 +2463,17 @@
       <c r="C73">
         <v>1</v>
       </c>
-      <c r="D73">
-        <v>2.809460693602245</v>
-      </c>
-      <c r="E73" t="s">
-        <v>111</v>
+      <c r="D73" t="s">
+        <v>105</v>
       </c>
       <c r="F73">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G73">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H73">
-        <v>0.9989979959919832</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2423,17 +2486,20 @@
       <c r="C74">
         <v>121</v>
       </c>
-      <c r="D74" t="s">
-        <v>105</v>
+      <c r="D74">
+        <v>0.01525721139318406</v>
+      </c>
+      <c r="E74" t="s">
+        <v>121</v>
       </c>
       <c r="F74">
-        <v>8.314049586776859</v>
+        <v>0.008264462809917356</v>
       </c>
       <c r="G74">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H74">
-        <v>-2.686952417231158</v>
+        <v>0.007262458801901323</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2450,13 +2516,13 @@
         <v>105</v>
       </c>
       <c r="F75">
-        <v>7.555555555555555</v>
+        <v>0</v>
       </c>
       <c r="G75">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H75">
-        <v>-3.445446448452461</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2473,13 +2539,13 @@
         <v>105</v>
       </c>
       <c r="F76">
-        <v>7.419354838709677</v>
+        <v>0</v>
       </c>
       <c r="G76">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H76">
-        <v>-3.58164716529834</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2496,13 +2562,13 @@
         <v>105</v>
       </c>
       <c r="F77">
-        <v>6.095238095238095</v>
+        <v>0</v>
       </c>
       <c r="G77">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H77">
-        <v>-4.905763908769922</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2519,13 +2585,13 @@
         <v>105</v>
       </c>
       <c r="F78">
-        <v>6.363636363636363</v>
+        <v>0</v>
       </c>
       <c r="G78">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H78">
-        <v>-4.637365640371653</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2542,13 +2608,13 @@
         <v>105</v>
       </c>
       <c r="F79">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G79">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H79">
-        <v>-4.001002004008017</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2565,13 +2631,13 @@
         <v>105</v>
       </c>
       <c r="F80">
-        <v>6.5</v>
+        <v>0</v>
       </c>
       <c r="G80">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H80">
-        <v>-4.501002004008017</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2584,20 +2650,17 @@
       <c r="C81">
         <v>1</v>
       </c>
-      <c r="D81">
-        <v>2.809460693602245</v>
-      </c>
-      <c r="E81" t="s">
-        <v>112</v>
+      <c r="D81" t="s">
+        <v>105</v>
       </c>
       <c r="F81">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G81">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H81">
-        <v>0.9989979959919832</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2610,17 +2673,20 @@
       <c r="C82">
         <v>457</v>
       </c>
-      <c r="D82" t="s">
-        <v>105</v>
+      <c r="D82">
+        <v>0.005006549770264956</v>
+      </c>
+      <c r="E82" t="s">
+        <v>122</v>
       </c>
       <c r="F82">
-        <v>10.30853391684902</v>
+        <v>0.002188183807439825</v>
       </c>
       <c r="G82">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H82">
-        <v>-0.6924680871590017</v>
+        <v>0.001186179799423793</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2633,17 +2699,20 @@
       <c r="C83">
         <v>180</v>
       </c>
-      <c r="D83" t="s">
-        <v>105</v>
+      <c r="D83">
+        <v>0.008433384132953879</v>
+      </c>
+      <c r="E83" t="s">
+        <v>123</v>
       </c>
       <c r="F83">
-        <v>8.838888888888889</v>
+        <v>0.005555555555555556</v>
       </c>
       <c r="G83">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H83">
-        <v>-2.162113115119128</v>
+        <v>0.004553551547539524</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2660,13 +2729,13 @@
         <v>105</v>
       </c>
       <c r="F84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G84">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H84">
-        <v>-10.00100200400802</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2683,13 +2752,13 @@
         <v>105</v>
       </c>
       <c r="F85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G85">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H85">
-        <v>-10.00100200400802</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2706,13 +2775,13 @@
         <v>105</v>
       </c>
       <c r="F86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G86">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H86">
-        <v>-10.00100200400802</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2729,13 +2798,13 @@
         <v>105</v>
       </c>
       <c r="F87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G87">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H87">
-        <v>-10.00100200400802</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2752,13 +2821,13 @@
         <v>105</v>
       </c>
       <c r="F88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G88">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H88">
-        <v>-10.00100200400802</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2775,13 +2844,13 @@
         <v>105</v>
       </c>
       <c r="F89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G89">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H89">
-        <v>-10.00100200400802</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2798,13 +2867,13 @@
         <v>105</v>
       </c>
       <c r="F90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G90">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H90">
-        <v>-10.00100200400802</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2821,13 +2890,13 @@
         <v>105</v>
       </c>
       <c r="F91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G91">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H91">
-        <v>-10.00100200400802</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2840,17 +2909,20 @@
       <c r="C92">
         <v>94</v>
       </c>
-      <c r="D92" t="s">
-        <v>105</v>
+      <c r="D92">
+        <v>0.01443939506571973</v>
+      </c>
+      <c r="E92" t="s">
+        <v>124</v>
       </c>
       <c r="F92">
-        <v>8.329787234042554</v>
+        <v>0.01063829787234043</v>
       </c>
       <c r="G92">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H92">
-        <v>-2.671214769965463</v>
+        <v>0.009636293864324394</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2867,13 +2939,13 @@
         <v>105</v>
       </c>
       <c r="F93">
-        <v>7.581818181818182</v>
+        <v>0</v>
       </c>
       <c r="G93">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H93">
-        <v>-3.419183822189835</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -2890,13 +2962,13 @@
         <v>105</v>
       </c>
       <c r="F94">
-        <v>7.4</v>
+        <v>0</v>
       </c>
       <c r="G94">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H94">
-        <v>-3.601002004008016</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -2913,13 +2985,13 @@
         <v>105</v>
       </c>
       <c r="F95">
-        <v>6.142857142857143</v>
+        <v>0</v>
       </c>
       <c r="G95">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H95">
-        <v>-4.858144861150874</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -2936,13 +3008,13 @@
         <v>105</v>
       </c>
       <c r="F96">
-        <v>2.714285714285714</v>
+        <v>0</v>
       </c>
       <c r="G96">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H96">
-        <v>-8.286716289722303</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -2959,13 +3031,13 @@
         <v>105</v>
       </c>
       <c r="F97">
-        <v>3.4</v>
+        <v>0</v>
       </c>
       <c r="G97">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H97">
-        <v>-7.601002004008016</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -2982,13 +3054,13 @@
         <v>105</v>
       </c>
       <c r="F98">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G98">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H98">
-        <v>-9.001002004008017</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -3005,13 +3077,13 @@
         <v>105</v>
       </c>
       <c r="F99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G99">
-        <v>11.00100200400802</v>
+        <v>0.001002004008016032</v>
       </c>
       <c r="H99">
-        <v>-10.00100200400802</v>
+        <v>-0.001002004008016032</v>
       </c>
     </row>
   </sheetData>

</xml_diff>